<commit_message>
Added swga enzyme selection
</commit_message>
<xml_diff>
--- a/templates/NOMADS_sWGA_Worksheet.xlsx
+++ b/templates/NOMADS_sWGA_Worksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\templates\Plasmodium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD644A4-F247-40D0-9110-9665EFD84732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BE8C29-E2D9-418F-AEAE-7E2CCA2B7642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" activeTab="3" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
@@ -24,8 +24,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Instructions!#REF!</definedName>
     <definedName name="exp_date">Assay!$C$2</definedName>
     <definedName name="exp_id">Assay!$C$5</definedName>
-    <definedName name="exp_notes">Assay!$C$13</definedName>
-    <definedName name="exp_rxns">Assay!$C$11</definedName>
+    <definedName name="exp_notes">Assay!$C$14</definedName>
+    <definedName name="exp_rxns">Assay!$C$12</definedName>
     <definedName name="exp_summary">Assay!$C$9</definedName>
     <definedName name="exp_type">reference!$B$7</definedName>
     <definedName name="exp_user">Assay!$C$3</definedName>
@@ -33,12 +33,13 @@
     <definedName name="export_folder">reference!$A$11</definedName>
     <definedName name="expt_summary">Assay!$C$9</definedName>
     <definedName name="expt_type">reference!$B$7</definedName>
-    <definedName name="swga_notes">Assay!$C$13</definedName>
-    <definedName name="swga_rxnvol">Assay!$C$12</definedName>
+    <definedName name="swga_enzyme">Assay!$C$11</definedName>
+    <definedName name="swga_notes">Assay!$C$14</definedName>
+    <definedName name="swga_rxnvol">Assay!$C$13</definedName>
     <definedName name="swga_targetmass">reference!$B$3</definedName>
     <definedName name="swga_template_maxvol">reference!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="236">
   <si>
     <t>ng</t>
   </si>
@@ -70,9 +71,6 @@
   </si>
   <si>
     <t>10mM dNTP</t>
-  </si>
-  <si>
-    <t>Phi29 (10U)</t>
   </si>
   <si>
     <t>Required fields</t>
@@ -708,9 +706,6 @@
   </si>
   <si>
     <t>Changelog from previous version</t>
-  </si>
-  <si>
-    <t>10x Phi29 Buffer</t>
   </si>
   <si>
     <t>100nM Primer Mix</t>
@@ -1002,9 +997,6 @@
     <t>Please contact the NOMADS team if any changes need to be made to the template.</t>
   </si>
   <si>
-    <t>Ability to filter sWGA table</t>
-  </si>
-  <si>
     <t>Person A</t>
   </si>
   <si>
@@ -1021,6 +1013,27 @@
   </si>
   <si>
     <t>PC</t>
+  </si>
+  <si>
+    <t>sWGA enzyme</t>
+  </si>
+  <si>
+    <t>DNA Polymerase</t>
+  </si>
+  <si>
+    <t>10x Buffer</t>
+  </si>
+  <si>
+    <t>phi29</t>
+  </si>
+  <si>
+    <t>equiphi29</t>
+  </si>
+  <si>
+    <t>swga_enzyme</t>
+  </si>
+  <si>
+    <t>Addition of swga enzyme capture</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1431,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1576,83 +1589,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1681,6 +1617,83 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1694,6 +1707,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2069,9 +2085,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FB4FA29E-6DC2-47A8-8DE8-3C1612926E90}" name="tbl_expt_metadata" displayName="tbl_expt_metadata" ref="A1:J2" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{FB4FA29E-6DC2-47A8-8DE8-3C1612926E90}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FB4FA29E-6DC2-47A8-8DE8-3C1612926E90}" name="tbl_expt_metadata" displayName="tbl_expt_metadata" ref="A1:K2" totalsRowShown="0">
+  <autoFilter ref="A1:K2" xr:uid="{FB4FA29E-6DC2-47A8-8DE8-3C1612926E90}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7A035B8A-404A-4AC3-B440-D82E5E6068A8}" name="expt_id">
       <calculatedColumnFormula>IF(LEN(exp_id)=0,"",exp_id)</calculatedColumnFormula>
     </tableColumn>
@@ -2095,6 +2111,9 @@
     </tableColumn>
     <tableColumn id="9" xr3:uid="{2D9B1B77-2E59-4E0D-ACB3-C21F2162AD9D}" name="expt_summary">
       <calculatedColumnFormula>IF(LEN(exp_summary)=0,"",exp_summary)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{00542FAB-A3C8-4C82-A468-72F2D2CB8137}" name="swga_enzyme">
+      <calculatedColumnFormula>swga_enzyme</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{D27AA281-2010-4088-B71D-18AD05E1377E}" name="swga_rxnvol_ul">
       <calculatedColumnFormula>IF(LEN(swga_rxnvol)=0,"",swga_rxnvol)</calculatedColumnFormula>
@@ -2435,10 +2454,10 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C11" sqref="C11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2447,992 +2466,1024 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="74" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
+      <c r="A1" s="69" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="71" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="70"/>
+      <c r="K2" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="62"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A3" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K3" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="60"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A4" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="72"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="K4" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="61"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="74"/>
+      <c r="C5" s="77" t="str">
+        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SW",VLOOKUP(C3,reference!G3:H7,2,FALSE),C4))</f>
+        <v/>
+      </c>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>183</v>
+      </c>
+      <c r="L5" s="79"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A6" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="75"/>
-      <c r="K2" s="86" t="s">
-        <v>138</v>
-      </c>
-      <c r="L2" s="86"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K3" s="84" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="84"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="26" t="s">
+      <c r="B6" s="74"/>
+      <c r="C6" s="85" t="str">
+        <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",CONCATENATE(C2,"_sWGA_",C5))</f>
+        <v/>
+      </c>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="23"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A7" s="89" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="89"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" t="s">
         <v>144</v>
       </c>
-      <c r="K4" s="85" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="85"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="76" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="80" t="str">
-        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SW",VLOOKUP(C3,reference!G3:H7,2,FALSE),C4))</f>
-        <v/>
-      </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="K5" s="82" t="s">
-        <v>184</v>
-      </c>
-      <c r="L5" s="82"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="76" t="s">
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A8" s="89" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="89"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A9" s="90" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="90"/>
+      <c r="C9" s="88" t="str">
+        <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
+        <v/>
+      </c>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A10" s="90" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" s="90"/>
+      <c r="C10" s="91" t="str">
+        <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary,".xlsx"))</f>
+        <v/>
+      </c>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A11" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="72"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="63" t="str">
-        <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",CONCATENATE(C2,"_sWGA_",C5))</f>
-        <v/>
-      </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="23"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="67" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="68" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="66" t="str">
-        <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
-        <v/>
-      </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="68" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="69" t="str">
-        <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary,".xlsx"))</f>
-        <v/>
-      </c>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="29"/>
-      <c r="B12" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" t="s">
-        <v>145</v>
+      <c r="B12" s="72"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="20" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="29"/>
       <c r="B13" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="91"/>
+        <v>151</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="29"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
+      <c r="B14" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="55">
-        <v>0.1</v>
-      </c>
+      <c r="A16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="14" t="str">
-        <f>CONCATENATE("  1. Make up master mix as below and add ", SUM(D19:D24), " µl to each well")</f>
-        <v xml:space="preserve">  1. Make up master mix as below and add -10 µl to each well</v>
+      <c r="A17" s="11" t="s">
+        <v>153</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="55">
+        <v>0.1</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A18" s="64" t="s">
+    <row r="18" spans="1:13">
+      <c r="A18" s="14" t="str">
+        <f>CONCATENATE("  1. Make up master mix as below and add ", SUM(D20:D25), " µl to each well")</f>
+        <v xml:space="preserve">  1. Make up master mix as below and add -10 µl to each well</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A19" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65" t="str">
+      <c r="E19" s="87"/>
+      <c r="F19" s="87" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="65"/>
-      <c r="J18" s="89" t="s">
+      <c r="G19" s="87"/>
+      <c r="J19" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="65"/>
+      <c r="L19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="89"/>
-      <c r="L18" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="71" t="s">
-        <v>201</v>
-      </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="70">
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="68">
         <f>swga_rxnvol/10</f>
         <v>0</v>
       </c>
-      <c r="E19" s="70"/>
-      <c r="F19" s="73" t="str">
-        <f t="shared" ref="F19:F22" si="0">IF(ISBLANK(swga_rxnvol),"",SUM(D19*exp_rxns*(1+$D$16)))</f>
-        <v/>
-      </c>
-      <c r="G19" s="73"/>
-      <c r="J19" s="90">
+      <c r="E20" s="68"/>
+      <c r="F20" s="83" t="str">
+        <f t="shared" ref="F20:F23" si="0">IF(ISBLANK(swga_rxnvol),"",SUM(D20*exp_rxns*(1+$D$17)))</f>
+        <v/>
+      </c>
+      <c r="G20" s="83"/>
+      <c r="J20" s="66">
         <v>35</v>
       </c>
-      <c r="K19" s="90"/>
-      <c r="L19" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="70">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="70"/>
-      <c r="F20" s="73" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G20" s="73"/>
-      <c r="J20" s="90">
-        <v>34</v>
-      </c>
-      <c r="K20" s="90"/>
+      <c r="K20" s="66"/>
       <c r="L20" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="59" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="70">
+      <c r="A21" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="68">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G21" s="83"/>
+      <c r="J21" s="66">
+        <v>34</v>
+      </c>
+      <c r="K21" s="66"/>
+      <c r="L21" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="81" t="s">
+        <v>200</v>
+      </c>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="68">
         <v>1.25</v>
       </c>
-      <c r="E21" s="70"/>
-      <c r="F21" s="73" t="str">
+      <c r="E22" s="68"/>
+      <c r="F22" s="83" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G21" s="73"/>
-      <c r="J21" s="87">
+      <c r="G22" s="83"/>
+      <c r="J22" s="63">
         <v>33</v>
       </c>
-      <c r="K21" s="87"/>
-      <c r="L21" s="6" t="s">
+      <c r="K22" s="63"/>
+      <c r="L22" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="68">
+        <v>5</v>
+      </c>
+      <c r="E23" s="68"/>
+      <c r="F23" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G23" s="83"/>
+      <c r="J23" s="64">
+        <v>32</v>
+      </c>
+      <c r="K23" s="64"/>
+      <c r="L23" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="70">
-        <v>5</v>
-      </c>
-      <c r="E22" s="70"/>
-      <c r="F22" s="73" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G22" s="73"/>
-      <c r="J22" s="88">
-        <v>32</v>
-      </c>
-      <c r="K22" s="88"/>
-      <c r="L22" s="7" t="s">
+    <row r="24" spans="1:13">
+      <c r="A24" s="96" t="str">
+        <f>IF(C11="","",C11)</f>
+        <v/>
+      </c>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="68">
+        <v>1</v>
+      </c>
+      <c r="E24" s="68"/>
+      <c r="F24" s="83" t="str">
+        <f>IF(ISBLANK(swga_rxnvol),"",SUM(D24*exp_rxns*(1+$D$17)))</f>
+        <v/>
+      </c>
+      <c r="G24" s="83"/>
+      <c r="J24" s="63">
+        <v>31</v>
+      </c>
+      <c r="K24" s="63"/>
+      <c r="L24" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="70">
-        <v>1</v>
-      </c>
-      <c r="E23" s="70"/>
-      <c r="F23" s="73" t="str">
-        <f>IF(ISBLANK(swga_rxnvol),"",SUM(D23*exp_rxns*(1+$D$16)))</f>
-        <v/>
-      </c>
-      <c r="G23" s="73"/>
-      <c r="J23" s="87">
-        <v>31</v>
-      </c>
-      <c r="K23" s="87"/>
-      <c r="L23" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="59" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="68">
+        <f>SUM(swga_rxnvol-swga_template_maxvol)-SUM(D20:E24)</f>
+        <v>-17.5</v>
+      </c>
+      <c r="E25" s="68"/>
+      <c r="F25" s="83" t="str">
+        <f>IF(ISBLANK(swga_rxnvol),"",SUM(D25*exp_rxns*(1+$D$17)))</f>
+        <v/>
+      </c>
+      <c r="G25" s="83"/>
+      <c r="J25" s="63">
+        <v>30</v>
+      </c>
+      <c r="K25" s="63"/>
+      <c r="L25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="70">
-        <f>SUM(swga_rxnvol-swga_template_maxvol)-SUM(D19:E23)</f>
-        <v>-17.5</v>
-      </c>
-      <c r="E24" s="70"/>
-      <c r="F24" s="73" t="str">
-        <f>IF(ISBLANK(swga_rxnvol),"",SUM(D24*exp_rxns*(1+$D$16)))</f>
-        <v/>
-      </c>
-      <c r="G24" s="73"/>
-      <c r="J24" s="87">
-        <v>30</v>
-      </c>
-      <c r="K24" s="87"/>
-      <c r="L24" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="G25" s="17" t="str">
-        <f>CONCATENATE("Add ",SUM(D19:D24)," µl of MM to each well")</f>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="G26" s="17" t="str">
+        <f>CONCATENATE("Add ",SUM(D20:D25)," µl of MM to each well")</f>
         <v>Add -10 µl of MM to each well</v>
       </c>
-      <c r="J25" s="87">
+      <c r="J26" s="63">
         <v>65</v>
       </c>
-      <c r="K25" s="87"/>
-      <c r="L25" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="B26" s="7"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="7"/>
-      <c r="G26" s="10"/>
-      <c r="J26" s="87">
-        <v>10</v>
-      </c>
-      <c r="K26" s="87"/>
-      <c r="L26" s="13" t="s">
-        <v>12</v>
+      <c r="K26" s="63"/>
+      <c r="L26" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="14" t="str">
-        <f>CONCATENATE("  2. For each sample add target of ",swga_targetmass," ng of DNA for each up to a max vol of ",swga_template_maxvol,"ul. Add TE as required.")</f>
-        <v xml:space="preserve">  2. For each sample add target of 40 ng of DNA for each up to a max vol of 10ul. Add TE as required.</v>
-      </c>
       <c r="B27" s="7"/>
       <c r="C27" s="9"/>
       <c r="D27" s="7"/>
-      <c r="F27" s="13"/>
       <c r="G27" s="10"/>
-      <c r="K27" s="83" t="s">
-        <v>147</v>
-      </c>
-      <c r="L27" s="83"/>
-      <c r="M27" s="83"/>
+      <c r="J27" s="63">
+        <v>10</v>
+      </c>
+      <c r="K27" s="63"/>
+      <c r="L27" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="14" t="s">
-        <v>155</v>
+      <c r="A28" s="14" t="str">
+        <f>CONCATENATE("  2. For each sample add target of ",swga_targetmass," ng of DNA for each up to a max vol of ",swga_template_maxvol,"ul. Add TE as required.")</f>
+        <v xml:space="preserve">  2. For each sample add target of 40 ng of DNA for each up to a max vol of 10ul. Add TE as required.</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="9"/>
       <c r="D28" s="7"/>
       <c r="F28" s="13"/>
       <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:13" ht="18.75">
+      <c r="K28" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="14" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="9"/>
       <c r="D29" s="7"/>
       <c r="F29" s="13"/>
       <c r="G29" s="10"/>
-      <c r="K29" s="83" t="s">
-        <v>147</v>
-      </c>
-      <c r="L29" s="83"/>
-      <c r="M29" s="83"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="14"/>
+    </row>
+    <row r="30" spans="1:13" ht="18.75">
+      <c r="A30" s="14" t="s">
+        <v>203</v>
+      </c>
       <c r="B30" s="7"/>
       <c r="C30" s="9"/>
       <c r="D30" s="7"/>
       <c r="F30" s="13"/>
       <c r="G30" s="10"/>
+      <c r="K30" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="7"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32"/>
-      <c r="B32" s="27">
+      <c r="A32" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33"/>
+      <c r="B33" s="27">
         <v>1</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C33" s="27">
         <v>2</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D33" s="27">
         <v>3</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E33" s="27">
         <v>4</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F33" s="27">
         <v>5</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G33" s="27">
         <v>6</v>
       </c>
-      <c r="H32" s="27">
+      <c r="H33" s="27">
         <v>7</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I33" s="27">
         <v>8</v>
       </c>
-      <c r="J32" s="27">
+      <c r="J33" s="27">
         <v>9</v>
       </c>
-      <c r="K32" s="27">
+      <c r="K33" s="27">
         <v>10</v>
       </c>
-      <c r="L32" s="27">
+      <c r="L33" s="27">
         <v>11</v>
       </c>
-      <c r="M32" s="27">
+      <c r="M33" s="27">
         <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D3),"",sWGA!$D3)</f>
-        <v/>
-      </c>
-      <c r="C33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D11),"",sWGA!$D11)</f>
-        <v/>
-      </c>
-      <c r="D33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D19),"",sWGA!$D19)</f>
-        <v/>
-      </c>
-      <c r="E33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D27),"",sWGA!$D27)</f>
-        <v/>
-      </c>
-      <c r="F33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D35),"",sWGA!$D35)</f>
-        <v/>
-      </c>
-      <c r="G33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D43),"",sWGA!$D43)</f>
-        <v/>
-      </c>
-      <c r="H33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D51),"",sWGA!$D51)</f>
-        <v/>
-      </c>
-      <c r="I33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D59),"",sWGA!$D59)</f>
-        <v/>
-      </c>
-      <c r="J33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D67),"",sWGA!$D67)</f>
-        <v/>
-      </c>
-      <c r="K33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D75),"",sWGA!$D75)</f>
-        <v/>
-      </c>
-      <c r="L33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D83),"",sWGA!$D83)</f>
-        <v/>
-      </c>
-      <c r="M33" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D91),"",sWGA!$D91)</f>
-        <v/>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D4),"",sWGA!$D4)</f>
+        <f>IF(ISBLANK(sWGA!$D3),"",sWGA!$D3)</f>
         <v/>
       </c>
       <c r="C34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D12),"",sWGA!$D12)</f>
+        <f>IF(ISBLANK(sWGA!$D11),"",sWGA!$D11)</f>
         <v/>
       </c>
       <c r="D34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D20),"",sWGA!$D20)</f>
+        <f>IF(ISBLANK(sWGA!$D19),"",sWGA!$D19)</f>
         <v/>
       </c>
       <c r="E34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D28),"",sWGA!$D28)</f>
+        <f>IF(ISBLANK(sWGA!$D27),"",sWGA!$D27)</f>
         <v/>
       </c>
       <c r="F34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D36),"",sWGA!$D36)</f>
+        <f>IF(ISBLANK(sWGA!$D35),"",sWGA!$D35)</f>
         <v/>
       </c>
       <c r="G34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D44),"",sWGA!$D44)</f>
+        <f>IF(ISBLANK(sWGA!$D43),"",sWGA!$D43)</f>
         <v/>
       </c>
       <c r="H34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D52),"",sWGA!$D52)</f>
+        <f>IF(ISBLANK(sWGA!$D51),"",sWGA!$D51)</f>
         <v/>
       </c>
       <c r="I34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D60),"",sWGA!$D60)</f>
+        <f>IF(ISBLANK(sWGA!$D59),"",sWGA!$D59)</f>
         <v/>
       </c>
       <c r="J34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D68),"",sWGA!$D68)</f>
+        <f>IF(ISBLANK(sWGA!$D67),"",sWGA!$D67)</f>
         <v/>
       </c>
       <c r="K34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D76),"",sWGA!$D76)</f>
+        <f>IF(ISBLANK(sWGA!$D75),"",sWGA!$D75)</f>
         <v/>
       </c>
       <c r="L34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D84),"",sWGA!$D84)</f>
+        <f>IF(ISBLANK(sWGA!$D83),"",sWGA!$D83)</f>
         <v/>
       </c>
       <c r="M34" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D92),"",sWGA!$D92)</f>
+        <f>IF(ISBLANK(sWGA!$D91),"",sWGA!$D91)</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D5),"",sWGA!$D5)</f>
+        <f>IF(ISBLANK(sWGA!$D4),"",sWGA!$D4)</f>
         <v/>
       </c>
       <c r="C35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D13),"",sWGA!$D13)</f>
+        <f>IF(ISBLANK(sWGA!$D12),"",sWGA!$D12)</f>
         <v/>
       </c>
       <c r="D35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D21),"",sWGA!$D21)</f>
+        <f>IF(ISBLANK(sWGA!$D20),"",sWGA!$D20)</f>
         <v/>
       </c>
       <c r="E35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D29),"",sWGA!$D29)</f>
+        <f>IF(ISBLANK(sWGA!$D28),"",sWGA!$D28)</f>
         <v/>
       </c>
       <c r="F35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D37),"",sWGA!$D37)</f>
+        <f>IF(ISBLANK(sWGA!$D36),"",sWGA!$D36)</f>
         <v/>
       </c>
       <c r="G35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D45),"",sWGA!$D45)</f>
+        <f>IF(ISBLANK(sWGA!$D44),"",sWGA!$D44)</f>
         <v/>
       </c>
       <c r="H35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D53),"",sWGA!$D53)</f>
+        <f>IF(ISBLANK(sWGA!$D52),"",sWGA!$D52)</f>
         <v/>
       </c>
       <c r="I35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D61),"",sWGA!$D61)</f>
+        <f>IF(ISBLANK(sWGA!$D60),"",sWGA!$D60)</f>
         <v/>
       </c>
       <c r="J35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D69),"",sWGA!$D69)</f>
+        <f>IF(ISBLANK(sWGA!$D68),"",sWGA!$D68)</f>
         <v/>
       </c>
       <c r="K35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D77),"",sWGA!$D77)</f>
+        <f>IF(ISBLANK(sWGA!$D76),"",sWGA!$D76)</f>
         <v/>
       </c>
       <c r="L35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D85),"",sWGA!$D85)</f>
+        <f>IF(ISBLANK(sWGA!$D84),"",sWGA!$D84)</f>
         <v/>
       </c>
       <c r="M35" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D93),"",sWGA!$D93)</f>
+        <f>IF(ISBLANK(sWGA!$D92),"",sWGA!$D92)</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D6),"",sWGA!$D6)</f>
+        <f>IF(ISBLANK(sWGA!$D5),"",sWGA!$D5)</f>
         <v/>
       </c>
       <c r="C36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D14),"",sWGA!$D14)</f>
+        <f>IF(ISBLANK(sWGA!$D13),"",sWGA!$D13)</f>
         <v/>
       </c>
       <c r="D36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D22),"",sWGA!$D22)</f>
+        <f>IF(ISBLANK(sWGA!$D21),"",sWGA!$D21)</f>
         <v/>
       </c>
       <c r="E36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D30),"",sWGA!$D30)</f>
+        <f>IF(ISBLANK(sWGA!$D29),"",sWGA!$D29)</f>
         <v/>
       </c>
       <c r="F36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D38),"",sWGA!$D38)</f>
+        <f>IF(ISBLANK(sWGA!$D37),"",sWGA!$D37)</f>
         <v/>
       </c>
       <c r="G36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D46),"",sWGA!$D46)</f>
+        <f>IF(ISBLANK(sWGA!$D45),"",sWGA!$D45)</f>
         <v/>
       </c>
       <c r="H36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D54),"",sWGA!$D54)</f>
+        <f>IF(ISBLANK(sWGA!$D53),"",sWGA!$D53)</f>
         <v/>
       </c>
       <c r="I36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D62),"",sWGA!$D62)</f>
+        <f>IF(ISBLANK(sWGA!$D61),"",sWGA!$D61)</f>
         <v/>
       </c>
       <c r="J36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D70),"",sWGA!$D70)</f>
+        <f>IF(ISBLANK(sWGA!$D69),"",sWGA!$D69)</f>
         <v/>
       </c>
       <c r="K36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D78),"",sWGA!$D78)</f>
+        <f>IF(ISBLANK(sWGA!$D77),"",sWGA!$D77)</f>
         <v/>
       </c>
       <c r="L36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D86),"",sWGA!$D86)</f>
+        <f>IF(ISBLANK(sWGA!$D85),"",sWGA!$D85)</f>
         <v/>
       </c>
       <c r="M36" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D94),"",sWGA!$D94)</f>
+        <f>IF(ISBLANK(sWGA!$D93),"",sWGA!$D93)</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D7),"",sWGA!$D7)</f>
+        <f>IF(ISBLANK(sWGA!$D6),"",sWGA!$D6)</f>
         <v/>
       </c>
       <c r="C37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D15),"",sWGA!$D15)</f>
+        <f>IF(ISBLANK(sWGA!$D14),"",sWGA!$D14)</f>
         <v/>
       </c>
       <c r="D37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D23),"",sWGA!$D23)</f>
+        <f>IF(ISBLANK(sWGA!$D22),"",sWGA!$D22)</f>
         <v/>
       </c>
       <c r="E37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D31),"",sWGA!$D31)</f>
+        <f>IF(ISBLANK(sWGA!$D30),"",sWGA!$D30)</f>
         <v/>
       </c>
       <c r="F37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D39),"",sWGA!$D39)</f>
+        <f>IF(ISBLANK(sWGA!$D38),"",sWGA!$D38)</f>
         <v/>
       </c>
       <c r="G37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D47),"",sWGA!$D47)</f>
+        <f>IF(ISBLANK(sWGA!$D46),"",sWGA!$D46)</f>
         <v/>
       </c>
       <c r="H37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D55),"",sWGA!$D55)</f>
+        <f>IF(ISBLANK(sWGA!$D54),"",sWGA!$D54)</f>
         <v/>
       </c>
       <c r="I37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D63),"",sWGA!$D63)</f>
+        <f>IF(ISBLANK(sWGA!$D62),"",sWGA!$D62)</f>
         <v/>
       </c>
       <c r="J37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D71),"",sWGA!$D71)</f>
+        <f>IF(ISBLANK(sWGA!$D70),"",sWGA!$D70)</f>
         <v/>
       </c>
       <c r="K37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D79),"",sWGA!$D79)</f>
+        <f>IF(ISBLANK(sWGA!$D78),"",sWGA!$D78)</f>
         <v/>
       </c>
       <c r="L37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D87),"",sWGA!$D87)</f>
+        <f>IF(ISBLANK(sWGA!$D86),"",sWGA!$D86)</f>
         <v/>
       </c>
       <c r="M37" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D95),"",sWGA!$D95)</f>
+        <f>IF(ISBLANK(sWGA!$D94),"",sWGA!$D94)</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D8),"",sWGA!$D8)</f>
+        <f>IF(ISBLANK(sWGA!$D7),"",sWGA!$D7)</f>
         <v/>
       </c>
       <c r="C38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D16),"",sWGA!$D16)</f>
+        <f>IF(ISBLANK(sWGA!$D15),"",sWGA!$D15)</f>
         <v/>
       </c>
       <c r="D38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D24),"",sWGA!$D24)</f>
+        <f>IF(ISBLANK(sWGA!$D23),"",sWGA!$D23)</f>
         <v/>
       </c>
       <c r="E38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D32),"",sWGA!$D32)</f>
+        <f>IF(ISBLANK(sWGA!$D31),"",sWGA!$D31)</f>
         <v/>
       </c>
       <c r="F38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D40),"",sWGA!$D40)</f>
+        <f>IF(ISBLANK(sWGA!$D39),"",sWGA!$D39)</f>
         <v/>
       </c>
       <c r="G38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D48),"",sWGA!$D48)</f>
+        <f>IF(ISBLANK(sWGA!$D47),"",sWGA!$D47)</f>
         <v/>
       </c>
       <c r="H38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D56),"",sWGA!$D56)</f>
+        <f>IF(ISBLANK(sWGA!$D55),"",sWGA!$D55)</f>
         <v/>
       </c>
       <c r="I38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D64),"",sWGA!$D64)</f>
+        <f>IF(ISBLANK(sWGA!$D63),"",sWGA!$D63)</f>
         <v/>
       </c>
       <c r="J38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D72),"",sWGA!$D72)</f>
+        <f>IF(ISBLANK(sWGA!$D71),"",sWGA!$D71)</f>
         <v/>
       </c>
       <c r="K38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D80),"",sWGA!$D80)</f>
+        <f>IF(ISBLANK(sWGA!$D79),"",sWGA!$D79)</f>
         <v/>
       </c>
       <c r="L38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D88),"",sWGA!$D88)</f>
+        <f>IF(ISBLANK(sWGA!$D87),"",sWGA!$D87)</f>
         <v/>
       </c>
       <c r="M38" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D96),"",sWGA!$D96)</f>
+        <f>IF(ISBLANK(sWGA!$D95),"",sWGA!$D95)</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D9),"",sWGA!$D9)</f>
+        <f>IF(ISBLANK(sWGA!$D8),"",sWGA!$D8)</f>
         <v/>
       </c>
       <c r="C39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D17),"",sWGA!$D17)</f>
+        <f>IF(ISBLANK(sWGA!$D16),"",sWGA!$D16)</f>
         <v/>
       </c>
       <c r="D39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D25),"",sWGA!$D25)</f>
+        <f>IF(ISBLANK(sWGA!$D24),"",sWGA!$D24)</f>
         <v/>
       </c>
       <c r="E39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D33),"",sWGA!$D33)</f>
+        <f>IF(ISBLANK(sWGA!$D32),"",sWGA!$D32)</f>
         <v/>
       </c>
       <c r="F39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D41),"",sWGA!$D41)</f>
+        <f>IF(ISBLANK(sWGA!$D40),"",sWGA!$D40)</f>
         <v/>
       </c>
       <c r="G39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D49),"",sWGA!$D49)</f>
+        <f>IF(ISBLANK(sWGA!$D48),"",sWGA!$D48)</f>
         <v/>
       </c>
       <c r="H39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D57),"",sWGA!$D57)</f>
+        <f>IF(ISBLANK(sWGA!$D56),"",sWGA!$D56)</f>
         <v/>
       </c>
       <c r="I39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D65),"",sWGA!$D65)</f>
+        <f>IF(ISBLANK(sWGA!$D64),"",sWGA!$D64)</f>
         <v/>
       </c>
       <c r="J39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D73),"",sWGA!$D73)</f>
+        <f>IF(ISBLANK(sWGA!$D72),"",sWGA!$D72)</f>
         <v/>
       </c>
       <c r="K39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D81),"",sWGA!$D81)</f>
+        <f>IF(ISBLANK(sWGA!$D80),"",sWGA!$D80)</f>
         <v/>
       </c>
       <c r="L39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D89),"",sWGA!$D89)</f>
+        <f>IF(ISBLANK(sWGA!$D88),"",sWGA!$D88)</f>
         <v/>
       </c>
       <c r="M39" s="32" t="str">
-        <f>IF(ISBLANK(sWGA!$D97),"",sWGA!$D97)</f>
+        <f>IF(ISBLANK(sWGA!$D96),"",sWGA!$D96)</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D9),"",sWGA!$D9)</f>
+        <v/>
+      </c>
+      <c r="C40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D17),"",sWGA!$D17)</f>
+        <v/>
+      </c>
+      <c r="D40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D25),"",sWGA!$D25)</f>
+        <v/>
+      </c>
+      <c r="E40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D33),"",sWGA!$D33)</f>
+        <v/>
+      </c>
+      <c r="F40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D41),"",sWGA!$D41)</f>
+        <v/>
+      </c>
+      <c r="G40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D49),"",sWGA!$D49)</f>
+        <v/>
+      </c>
+      <c r="H40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D57),"",sWGA!$D57)</f>
+        <v/>
+      </c>
+      <c r="I40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D65),"",sWGA!$D65)</f>
+        <v/>
+      </c>
+      <c r="J40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D73),"",sWGA!$D73)</f>
+        <v/>
+      </c>
+      <c r="K40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D81),"",sWGA!$D81)</f>
+        <v/>
+      </c>
+      <c r="L40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D89),"",sWGA!$D89)</f>
+        <v/>
+      </c>
+      <c r="M40" s="32" t="str">
+        <f>IF(ISBLANK(sWGA!$D97),"",sWGA!$D97)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D10),"",sWGA!$D10)</f>
         <v/>
       </c>
-      <c r="C40" s="32" t="str">
+      <c r="C41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D18),"",sWGA!$D18)</f>
         <v/>
       </c>
-      <c r="D40" s="32" t="str">
+      <c r="D41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D26),"",sWGA!$D26)</f>
         <v/>
       </c>
-      <c r="E40" s="32" t="str">
+      <c r="E41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D34),"",sWGA!$D34)</f>
         <v/>
       </c>
-      <c r="F40" s="32" t="str">
+      <c r="F41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D42),"",sWGA!$D42)</f>
         <v/>
       </c>
-      <c r="G40" s="32" t="str">
+      <c r="G41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D50),"",sWGA!$D50)</f>
         <v/>
       </c>
-      <c r="H40" s="32" t="str">
+      <c r="H41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D58),"",sWGA!$D58)</f>
         <v/>
       </c>
-      <c r="I40" s="32" t="str">
+      <c r="I41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D66),"",sWGA!$D66)</f>
         <v/>
       </c>
-      <c r="J40" s="32" t="str">
+      <c r="J41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D74),"",sWGA!$D74)</f>
         <v/>
       </c>
-      <c r="K40" s="32" t="str">
+      <c r="K41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D82),"",sWGA!$D82)</f>
         <v/>
       </c>
-      <c r="L40" s="32" t="str">
+      <c r="L41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D90),"",sWGA!$D90)</f>
         <v/>
       </c>
-      <c r="M40" s="32" t="str">
+      <c r="M41" s="32" t="str">
         <f>IF(ISBLANK(sWGA!$D98),"",sWGA!$D98)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="7"/>
+    <row r="42" spans="1:13">
+      <c r="A42" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="60">
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="C13:K14"/>
+  <mergeCells count="62">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:B3"/>
@@ -3445,41 +3496,25 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="K5:L6"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="C14:K15"/>
+    <mergeCell ref="D25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C4 C11:C13">
+  <conditionalFormatting sqref="C2:C4 C11:C14">
     <cfRule type="expression" dxfId="4" priority="15">
       <formula>COUNTIF(C2,"")</formula>
     </cfRule>
@@ -3489,9 +3524,9 @@
       <formula>COUNTIF(C7,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="D17">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>COUNTIF(D16,"")</formula>
+      <formula>COUNTIF(D17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -3504,12 +3539,12 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85B9980E-D072-4E08-B792-4B86FA663CD4}">
           <x14:formula1>
             <xm:f>reference!$E$3:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C12</xm:sqref>
+          <xm:sqref>C13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECC56CCB-ED86-47E8-A451-039865410494}">
           <x14:formula1>
@@ -3522,6 +3557,12 @@
             <xm:f>reference!$G$3:$G$7</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49BACFA1-87AC-4545-9963-95B02395023D}">
+          <x14:formula1>
+            <xm:f>reference!$E$7:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C11:F11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3556,7 +3597,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="C1" s="92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="93"/>
       <c r="E1" s="94" t="s">
@@ -3570,34 +3611,34 @@
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="48.75" customHeight="1">
       <c r="A2" s="54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="45" t="s">
+      <c r="I2" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="I2" s="45" t="s">
-        <v>157</v>
-      </c>
       <c r="J2" s="45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
@@ -3605,7 +3646,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="39"/>
@@ -3627,7 +3668,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="39"/>
@@ -3649,7 +3690,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="39"/>
@@ -3671,7 +3712,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="39"/>
@@ -3693,7 +3734,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="39"/>
@@ -3715,7 +3756,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="39"/>
@@ -3737,7 +3778,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="39"/>
@@ -3759,7 +3800,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="39"/>
@@ -3781,7 +3822,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="39"/>
@@ -3803,7 +3844,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="39"/>
@@ -3825,7 +3866,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="39"/>
@@ -3847,7 +3888,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="39"/>
@@ -3869,7 +3910,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="39"/>
@@ -3891,7 +3932,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="39"/>
@@ -3913,7 +3954,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="39"/>
@@ -3935,7 +3976,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="39"/>
@@ -3957,7 +3998,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="39"/>
@@ -3979,7 +4020,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="39"/>
@@ -4001,7 +4042,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="39"/>
@@ -4023,7 +4064,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="39"/>
@@ -4045,7 +4086,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="39"/>
@@ -4067,7 +4108,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="39"/>
@@ -4089,7 +4130,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="39"/>
@@ -4111,7 +4152,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="39"/>
@@ -4133,7 +4174,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="39"/>
@@ -4155,7 +4196,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="39"/>
@@ -4177,7 +4218,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="39"/>
@@ -4199,7 +4240,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="39"/>
@@ -4221,7 +4262,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="39"/>
@@ -4243,7 +4284,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="39"/>
@@ -4265,7 +4306,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="39"/>
@@ -4287,7 +4328,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="39"/>
@@ -4309,7 +4350,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="39"/>
@@ -4331,7 +4372,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="30"/>
       <c r="D36" s="39"/>
@@ -4353,7 +4394,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="39"/>
@@ -4375,7 +4416,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="39"/>
@@ -4397,7 +4438,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="39"/>
@@ -4419,7 +4460,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="39"/>
@@ -4441,7 +4482,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C41" s="30"/>
       <c r="D41" s="39"/>
@@ -4463,7 +4504,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="30"/>
       <c r="D42" s="39"/>
@@ -4485,7 +4526,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="30"/>
       <c r="D43" s="39"/>
@@ -4507,7 +4548,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="39"/>
@@ -4529,7 +4570,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="39"/>
@@ -4551,7 +4592,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46" s="30"/>
       <c r="D46" s="39"/>
@@ -4573,7 +4614,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="39"/>
@@ -4595,7 +4636,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48" s="30"/>
       <c r="D48" s="39"/>
@@ -4617,7 +4658,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" s="30"/>
       <c r="D49" s="39"/>
@@ -4639,7 +4680,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50" s="30"/>
       <c r="D50" s="39"/>
@@ -4661,7 +4702,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="39"/>
@@ -4683,7 +4724,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="30"/>
       <c r="D52" s="39"/>
@@ -4705,7 +4746,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="30"/>
       <c r="D53" s="39"/>
@@ -4727,7 +4768,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54" s="30"/>
       <c r="D54" s="39"/>
@@ -4749,7 +4790,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="39"/>
@@ -4771,7 +4812,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" s="30"/>
       <c r="D56" s="39"/>
@@ -4793,7 +4834,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C57" s="30"/>
       <c r="D57" s="39"/>
@@ -4815,7 +4856,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" s="30"/>
       <c r="D58" s="39"/>
@@ -4837,7 +4878,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="39"/>
@@ -4859,7 +4900,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C60" s="30"/>
       <c r="D60" s="39"/>
@@ -4881,7 +4922,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C61" s="30"/>
       <c r="D61" s="39"/>
@@ -4903,7 +4944,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C62" s="30"/>
       <c r="D62" s="39"/>
@@ -4925,7 +4966,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C63" s="30"/>
       <c r="D63" s="39"/>
@@ -4947,7 +4988,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C64" s="30"/>
       <c r="D64" s="39"/>
@@ -4969,7 +5010,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C65" s="30"/>
       <c r="D65" s="39"/>
@@ -4991,7 +5032,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C66" s="30"/>
       <c r="D66" s="39"/>
@@ -5013,7 +5054,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C67" s="30"/>
       <c r="D67" s="39"/>
@@ -5035,7 +5076,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C68" s="30"/>
       <c r="D68" s="39"/>
@@ -5057,7 +5098,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C69" s="30"/>
       <c r="D69" s="39"/>
@@ -5079,7 +5120,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="39"/>
@@ -5101,7 +5142,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C71" s="30"/>
       <c r="D71" s="39"/>
@@ -5123,7 +5164,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C72" s="30"/>
       <c r="D72" s="39"/>
@@ -5145,7 +5186,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C73" s="30"/>
       <c r="D73" s="39"/>
@@ -5167,7 +5208,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C74" s="30"/>
       <c r="D74" s="39"/>
@@ -5189,7 +5230,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C75" s="30"/>
       <c r="D75" s="39"/>
@@ -5211,7 +5252,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C76" s="30"/>
       <c r="D76" s="39"/>
@@ -5233,7 +5274,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C77" s="30"/>
       <c r="D77" s="39"/>
@@ -5255,7 +5296,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C78" s="30"/>
       <c r="D78" s="39"/>
@@ -5277,7 +5318,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C79" s="30"/>
       <c r="D79" s="39"/>
@@ -5299,7 +5340,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C80" s="30"/>
       <c r="D80" s="39"/>
@@ -5321,7 +5362,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C81" s="30"/>
       <c r="D81" s="39"/>
@@ -5343,7 +5384,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C82" s="30"/>
       <c r="D82" s="39"/>
@@ -5365,7 +5406,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C83" s="30"/>
       <c r="D83" s="39"/>
@@ -5387,7 +5428,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C84" s="30"/>
       <c r="D84" s="39"/>
@@ -5409,7 +5450,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="39"/>
@@ -5431,7 +5472,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C86" s="30"/>
       <c r="D86" s="39"/>
@@ -5453,7 +5494,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C87" s="30"/>
       <c r="D87" s="39"/>
@@ -5475,7 +5516,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C88" s="30"/>
       <c r="D88" s="39"/>
@@ -5497,7 +5538,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C89" s="30"/>
       <c r="D89" s="39"/>
@@ -5519,7 +5560,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C90" s="30"/>
       <c r="D90" s="39"/>
@@ -5541,7 +5582,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C91" s="30"/>
       <c r="D91" s="39"/>
@@ -5563,7 +5604,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C92" s="30"/>
       <c r="D92" s="39"/>
@@ -5585,7 +5626,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C93" s="30"/>
       <c r="D93" s="39"/>
@@ -5607,7 +5648,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C94" s="30"/>
       <c r="D94" s="39"/>
@@ -5629,7 +5670,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C95" s="30"/>
       <c r="D95" s="39"/>
@@ -5651,7 +5692,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C96" s="30"/>
       <c r="D96" s="39"/>
@@ -5673,7 +5714,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C97" s="30"/>
       <c r="D97" s="39"/>
@@ -5695,7 +5736,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C98" s="30"/>
       <c r="D98" s="39"/>
@@ -5908,7 +5949,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5930,34 +5971,34 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1">
       <c r="A2" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="E2" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>142</v>
-      </c>
       <c r="J2" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="37">
         <v>40</v>
@@ -5969,105 +6010,114 @@
         <v>30</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B4" s="38">
         <v>10</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="37">
         <v>50</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75">
       <c r="E5" s="4"/>
       <c r="G5" s="36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="16.5" thickBot="1">
       <c r="A6" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
+      <c r="E6" s="24" t="s">
+        <v>230</v>
+      </c>
       <c r="G6" s="36"/>
       <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>232</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>233</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="G9" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="16.5" thickBot="1">
       <c r="A10" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="G12" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -6075,6 +6125,7 @@
       <c r="N12" s="3"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6086,7 +6137,9 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5"/>
   <cols>
@@ -6102,12 +6155,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="46.5">
       <c r="A1" s="52" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="48" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6115,93 +6168,93 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="46" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="47" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B11" s="48"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="47" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="48" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="48" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="48" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="48" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -6209,17 +6262,17 @@
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="46" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="47" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -6233,52 +6286,55 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="8" width="16.125" customWidth="1"/>
-    <col min="9" max="9" width="18.875" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="1" max="9" width="16.125" customWidth="1"/>
+    <col min="10" max="10" width="18.875" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
         <v>173</v>
       </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F1" t="s">
-        <v>175</v>
-      </c>
       <c r="G1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" t="s">
         <v>160</v>
       </c>
-      <c r="J1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="str">
         <f>IF(LEN(exp_id)=0,"",exp_id)</f>
         <v/>
@@ -6297,7 +6353,7 @@
       </c>
       <c r="E2">
         <f>IF(LEN(exp_version)=0,"",exp_version)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" t="str">
         <f>IF(LEN(exp_rxns)=0,"",exp_rxns)</f>
@@ -6311,17 +6367,21 @@
         <f>IF(LEN(exp_summary)=0,"",exp_summary)</f>
         <v/>
       </c>
-      <c r="I2" t="str">
+      <c r="I2">
+        <f>swga_enzyme</f>
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
         <f>IF(LEN(swga_rxnvol)=0,"",swga_rxnvol)</f>
         <v/>
       </c>
-      <c r="J2">
+      <c r="K2">
         <f>IF(LEN(swga_targetmass)=0,"",swga_targetmass)</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MdJATUqKFoAcT0nd7E0Eso0OUUv+PvS9cO/adsidY8Hz5f81ZMuL73JBUiuxigJW2EiT3bDWxP07Uk7KG0JD1A==" saltValue="dUEvDhlHGdkEHcej9awLlg==" spinCount="100000" sheet="1" scenarios="1" formatColumns="0" insertRows="0" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tDcrRq4wnjvk/XNE0KlG9X1Y0ZMU7FkLxcMq6SYhRbf4l5KeeZE5iy/NQ043rCKPXQ6532BBkrBRwBm4vOOJmg==" saltValue="H2ijzumCfyyiA1dSXFCSgQ==" spinCount="100000" sheet="1" scenarios="1" formatColumns="0" insertRows="0" autoFilter="0"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6353,22 +6413,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
         <v>162</v>
       </c>
-      <c r="B1" t="s">
-        <v>163</v>
-      </c>
       <c r="C1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
         <v>168</v>
-      </c>
-      <c r="F1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
Removed some data that was inadvertantly left
</commit_message>
<xml_diff>
--- a/templates/NOMADS_sWGA_Worksheet.xlsx
+++ b/templates/NOMADS_sWGA_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B1080D-6F36-441F-84BE-EB84BD39715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3557548-B6CA-45A5-A7BE-06821607D948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46284" windowHeight="23172" activeTab="2" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17532" activeTab="1" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="6" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="229">
   <si>
     <t>ng</t>
   </si>
@@ -846,12 +846,6 @@
   </si>
   <si>
     <t>Copy these columns to the PCR template</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1683,6 +1677,114 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1696,103 +1798,11 @@
     <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1819,22 +1829,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1847,33 +1841,6 @@
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="1"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2110,6 +2077,33 @@
         </bottom>
       </border>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="1"/>
     </dxf>
     <dxf>
       <font>
@@ -2371,37 +2365,37 @@
     <tableColumn id="2" xr3:uid="{CE61E1E1-E9B3-4D58-9DFE-1AB6DDFCD05A}" name="Sample ID" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{9795EF0E-2DE1-455A-A3FF-0804F7CBA8C3}" name="Extraction ID" dataDxfId="25"/>
     <tableColumn id="4" xr3:uid="{5587DAF9-72AA-46A4-AAFA-83520030B12F}" name="Sample Type" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{AE7E794D-3E11-4B03-8051-B54164DF087E}" name="sWGA Identifier" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{AE7E794D-3E11-4B03-8051-B54164DF087E}" name="sWGA Identifier" dataDxfId="23">
       <calculatedColumnFormula>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{17E17A49-9A1B-4B36-98B0-66368F2A095E}" name="sWGA template (ul)" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{6392E74F-2A5C-4E61-A4E5-54FD59E2FF90}" name="sWGA qubit [DNA] (ng / ul)" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{182C6360-B664-4CDB-83F5-523D173848EB}" name="sWGA Dilution Factor" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{B3E809FC-AA96-4329-8BC3-6D3188F7C694}" name="sWGA product [DNA] (ng / ul)" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{17E17A49-9A1B-4B36-98B0-66368F2A095E}" name="sWGA template (ul)" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{6392E74F-2A5C-4E61-A4E5-54FD59E2FF90}" name="sWGA qubit [DNA] (ng / ul)" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{182C6360-B664-4CDB-83F5-523D173848EB}" name="sWGA Dilution Factor" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{B3E809FC-AA96-4329-8BC3-6D3188F7C694}" name="sWGA product [DNA] (ng / ul)" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(tbl_sWGA[[#This Row],[sWGA qubit '[DNA'] (ng / ul)]]),ISBLANK(tbl_sWGA[[#This Row],[sWGA Dilution Factor]])),"",SUM(tbl_sWGA[[#This Row],[sWGA qubit '[DNA'] (ng / ul)]]*tbl_sWGA[[#This Row],[sWGA Dilution Factor]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1D653C53-7C54-49A7-9A0B-EB787729497D}" name="Proceed with PCR" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{1D653C53-7C54-49A7-9A0B-EB787729497D}" name="Proceed with PCR" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{736B7BD8-BF8D-47BE-8721-6207502377C8}" name="Table2" displayName="Table2" ref="I16:J26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{736B7BD8-BF8D-47BE-8721-6207502377C8}" name="Table2" displayName="Table2" ref="I16:J26" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16">
   <autoFilter ref="I16:J26" xr:uid="{736B7BD8-BF8D-47BE-8721-6207502377C8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{79224628-9936-4F26-8939-9F356DA22897}" name="User" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{9E13A328-1D21-445A-A3C8-FEEC88F75FCB}" name="Initials" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{79224628-9936-4F26-8939-9F356DA22897}" name="User" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{9E13A328-1D21-445A-A3C8-FEEC88F75FCB}" name="Initials" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72AF3EEB-AE70-42E3-B795-B0DBD63BB741}" name="Table5" displayName="Table5" ref="L16:L26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72AF3EEB-AE70-42E3-B795-B0DBD63BB741}" name="Table5" displayName="Table5" ref="L16:L26" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
   <autoFilter ref="L16:L26" xr:uid="{72AF3EEB-AE70-42E3-B795-B0DBD63BB741}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C86FE0A5-E4CA-44A1-8211-F65CA137B446}" name="Project" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{C86FE0A5-E4CA-44A1-8211-F65CA137B446}" name="Project" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2459,10 +2453,10 @@
     <tableColumn id="3" xr3:uid="{E11C4165-C164-4B88-9BF1-7FC2458E8999}" name="extraction_id">
       <calculatedColumnFormula>IF(LEN(sWGA!F4)=0,"",sWGA!F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1FB0E1F2-B22B-4383-B21B-4C2C979A2F8D}" name="sample_type" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{1FB0E1F2-B22B-4383-B21B-4C2C979A2F8D}" name="sample_type" dataDxfId="8">
       <calculatedColumnFormula>IF(LEN(sWGA!G4)=0,"",sWGA!G4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{D54B2CD4-28CD-4925-BA77-787E61BD2826}" name="expt_id" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{D54B2CD4-28CD-4925-BA77-787E61BD2826}" name="expt_id" dataDxfId="7">
       <calculatedColumnFormula>IF(LEN(sWGA!H4)=0,"",exp_id)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F5CC8E00-1DA6-4870-97ED-B9F5BA34367D}" name="swga_identifier">
@@ -2792,190 +2786,190 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="87" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="106" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="106"/>
-      <c r="K2" s="114" t="s">
+      <c r="H2" s="88"/>
+      <c r="K2" s="98" t="s">
         <v>136</v>
       </c>
-      <c r="L2" s="114"/>
+      <c r="L2" s="98"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
       <c r="G3" t="s">
         <v>143</v>
       </c>
-      <c r="K3" s="115" t="s">
+      <c r="K3" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="115"/>
+      <c r="L3" s="99"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
       <c r="G4" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="K4" s="116" t="s">
+      <c r="K4" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="116"/>
+      <c r="L4" s="100"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="108"/>
-      <c r="C5" s="111" t="str">
+      <c r="B5" s="92"/>
+      <c r="C5" s="95" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SW",VLOOKUP(C3,Reference!I17:J24,2,FALSE),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
       <c r="G5" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="K5" s="113" t="s">
+      <c r="K5" s="97" t="s">
         <v>177</v>
       </c>
-      <c r="L5" s="113"/>
+      <c r="L5" s="97"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="91" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="117" t="str">
+      <c r="B6" s="92"/>
+      <c r="C6" s="101" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",CONCATENATE(C2,"_sWGA_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
       <c r="G6" s="23"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="114" t="s">
         <v>178</v>
       </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="115"/>
       <c r="G7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="114" t="s">
         <v>179</v>
       </c>
-      <c r="B8" s="98"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="115"/>
       <c r="G8" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="96" t="s">
+      <c r="A9" s="112" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="97" t="str">
+      <c r="B9" s="112"/>
+      <c r="C9" s="113" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="97"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="20" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="112" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="86" t="str">
+      <c r="B10" s="112"/>
+      <c r="C10" s="119" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
       <c r="G11" t="s">
         <v>143</v>
       </c>
       <c r="H11"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="89" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
       <c r="G12" s="20" t="s">
         <v>148</v>
       </c>
@@ -2985,13 +2979,13 @@
       <c r="B13" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="100">
+      <c r="C13" s="110">
         <f>IF(swga_enzyme=Reference!$E$17,50,20)</f>
         <v>20</v>
       </c>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
       <c r="G13"/>
     </row>
     <row r="14" spans="1:13">
@@ -3059,181 +3053,181 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:13" ht="16.2" thickBot="1">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="93"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="94" t="s">
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94" t="str">
+      <c r="E19" s="105"/>
+      <c r="F19" s="105" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G19" s="94"/>
-      <c r="J19" s="102" t="s">
+      <c r="G19" s="105"/>
+      <c r="J19" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="102"/>
+      <c r="K19" s="103"/>
       <c r="L19" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="109" t="s">
         <v>201</v>
       </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="90">
+      <c r="B20" s="109"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="106">
         <f>swga_rxnvol/10</f>
         <v>2</v>
       </c>
-      <c r="E20" s="90"/>
-      <c r="F20" s="101">
+      <c r="E20" s="106"/>
+      <c r="F20" s="111">
         <f t="shared" ref="F20:F23" si="0">IF(ISBLANK(swga_rxnvol),"",SUM(D20*exp_rxns*(1+$D$17)))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="101"/>
-      <c r="J20" s="103">
+      <c r="G20" s="111"/>
+      <c r="J20" s="102">
         <f>Reference!E26</f>
         <v>45</v>
       </c>
-      <c r="K20" s="103"/>
+      <c r="K20" s="102"/>
       <c r="L20" s="10" t="str">
         <f>Reference!F26</f>
         <v>Prepare</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="92" t="str">
+      <c r="A21" s="107" t="str">
         <f>IF(swga_enzyme=Reference!$E$17,"100nM Primer Mix","500uM Primer Mix")</f>
         <v>500uM Primer Mix</v>
       </c>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="90">
+      <c r="B21" s="107"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="106">
         <f>IF(swga_enzyme=Reference!$E$17,0.25,2)</f>
         <v>2</v>
       </c>
-      <c r="E21" s="90"/>
-      <c r="F21" s="101">
+      <c r="E21" s="106"/>
+      <c r="F21" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="101"/>
-      <c r="J21" s="103">
+      <c r="G21" s="111"/>
+      <c r="J21" s="102">
         <f>Reference!E27</f>
         <v>45</v>
       </c>
-      <c r="K21" s="103"/>
+      <c r="K21" s="102"/>
       <c r="L21" s="10" t="str">
         <f>Reference!F27</f>
         <v>60 min</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="92" t="str">
+      <c r="A22" s="107" t="str">
         <f>IF(swga_enzyme=Reference!$E$17,"BSA (20mg/mL)","DTT")</f>
         <v>DTT</v>
       </c>
-      <c r="B22" s="92"/>
-      <c r="C22" s="92"/>
-      <c r="D22" s="90">
+      <c r="B22" s="107"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="106">
         <f>IF(swga_enzyme=Reference!$E$17,1.25,0.2)</f>
         <v>0.2</v>
       </c>
-      <c r="E22" s="90"/>
-      <c r="F22" s="101">
+      <c r="E22" s="106"/>
+      <c r="F22" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="101"/>
-      <c r="J22" s="103">
+      <c r="G22" s="111"/>
+      <c r="J22" s="102">
         <f>Reference!E28</f>
         <v>65</v>
       </c>
-      <c r="K22" s="103"/>
+      <c r="K22" s="102"/>
       <c r="L22" s="10" t="str">
         <f>Reference!F28</f>
         <v>10 min</v>
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="91" t="s">
+      <c r="A23" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="90">
+      <c r="B23" s="109"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="106">
         <f>IF(swga_enzyme=Reference!$E$17,5,2)</f>
         <v>2</v>
       </c>
-      <c r="E23" s="90"/>
-      <c r="F23" s="101">
+      <c r="E23" s="106"/>
+      <c r="F23" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="101"/>
-      <c r="J23" s="103">
+      <c r="G23" s="111"/>
+      <c r="J23" s="102">
         <f>Reference!E29</f>
         <v>8</v>
       </c>
-      <c r="K23" s="103"/>
+      <c r="K23" s="102"/>
       <c r="L23" s="10" t="str">
         <f>Reference!F29</f>
         <v>∞</v>
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="99" t="str">
+      <c r="A24" s="108" t="str">
         <f>_xlfn.CONCAT(IF(C11="","Select",C11)," polymerase")</f>
         <v>Select polymerase</v>
       </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
-      <c r="D24" s="90">
+      <c r="B24" s="109"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="106">
         <v>1</v>
       </c>
-      <c r="E24" s="90"/>
-      <c r="F24" s="101">
+      <c r="E24" s="106"/>
+      <c r="F24" s="111">
         <f>IF(ISBLANK(swga_rxnvol),"",SUM(D24*exp_rxns*(1+$D$17)))</f>
         <v>0</v>
       </c>
-      <c r="G24" s="101"/>
-      <c r="J24" s="103" t="str">
+      <c r="G24" s="111"/>
+      <c r="J24" s="102" t="str">
         <f>Reference!E30</f>
         <v>-</v>
       </c>
-      <c r="K24" s="103"/>
+      <c r="K24" s="102"/>
       <c r="L24" s="10" t="str">
         <f>Reference!F30</f>
         <v>-</v>
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="90">
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="106">
         <f>SUM(swga_rxnvol-swga_template_maxvol)-SUM(D20:E24)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="90"/>
-      <c r="F25" s="101">
+      <c r="E25" s="106"/>
+      <c r="F25" s="111">
         <f>IF(ISBLANK(swga_rxnvol),"",SUM(D25*exp_rxns*(1+$D$17)))</f>
         <v>0</v>
       </c>
-      <c r="G25" s="101"/>
-      <c r="J25" s="103" t="str">
+      <c r="G25" s="111"/>
+      <c r="J25" s="102" t="str">
         <f>Reference!E31</f>
         <v>-</v>
       </c>
-      <c r="K25" s="103"/>
+      <c r="K25" s="102"/>
       <c r="L25" s="10" t="str">
         <f>Reference!F31</f>
         <v>-</v>
@@ -3244,11 +3238,11 @@
         <f>CONCATENATE("Add ",SUM(D20:D25)," µl of MM to each well")</f>
         <v>Add 7.2 µl of MM to each well</v>
       </c>
-      <c r="J26" s="103" t="str">
+      <c r="J26" s="102" t="str">
         <f>Reference!E32</f>
         <v>-</v>
       </c>
-      <c r="K26" s="103"/>
+      <c r="K26" s="102"/>
       <c r="L26" s="10" t="str">
         <f>Reference!F32</f>
         <v>-</v>
@@ -3259,11 +3253,11 @@
       <c r="C27" s="9"/>
       <c r="D27" s="7"/>
       <c r="G27" s="10"/>
-      <c r="J27" s="103" t="str">
+      <c r="J27" s="102" t="str">
         <f>Reference!E33</f>
         <v>-</v>
       </c>
-      <c r="K27" s="103"/>
+      <c r="K27" s="102"/>
       <c r="L27" s="10" t="str">
         <f>Reference!F33</f>
         <v>-</v>
@@ -3279,11 +3273,11 @@
       <c r="D28" s="7"/>
       <c r="F28" s="13"/>
       <c r="G28" s="10"/>
-      <c r="K28" s="84" t="s">
+      <c r="K28" s="117" t="s">
         <v>145</v>
       </c>
-      <c r="L28" s="84"/>
-      <c r="M28" s="84"/>
+      <c r="L28" s="117"/>
+      <c r="M28" s="117"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="14" t="s">
@@ -3296,25 +3290,25 @@
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:13" ht="33" customHeight="1">
-      <c r="A30" s="95" t="str">
+      <c r="A30" s="121" t="str">
         <f>IF(swga_enzyme=Reference!$E$17,"  4. Quantify 1 µl (199 µl WS 1X HS DNA). Dilute in water if required","  4. Dilute sWGA product by adding 160 µl water or low TE-Buffer (mix well). Aliquot 90 µl into backup plate and store at 4°C")</f>
         <v xml:space="preserve">  4. Dilute sWGA product by adding 160 µl water or low TE-Buffer (mix well). Aliquot 90 µl into backup plate and store at 4°C</v>
       </c>
-      <c r="B30" s="95"/>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95"/>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="85" t="str">
+      <c r="B30" s="121"/>
+      <c r="C30" s="121"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="121"/>
+      <c r="G30" s="121"/>
+      <c r="H30" s="121"/>
+      <c r="I30" s="121"/>
+      <c r="J30" s="121"/>
+      <c r="K30" s="118" t="str">
         <f>IF(swga_enzyme=Reference!$E$17,"(Enter in sWGA Tab)","")</f>
         <v/>
       </c>
-      <c r="L30" s="85"/>
-      <c r="M30" s="85"/>
+      <c r="L30" s="118"/>
+      <c r="M30" s="118"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="14" t="str">
@@ -3326,12 +3320,12 @@
       <c r="D31" s="7"/>
       <c r="F31" s="13"/>
       <c r="G31" s="10"/>
-      <c r="K31" s="85" t="str">
+      <c r="K31" s="118" t="str">
         <f>IF(swga_enzyme=Reference!$E$17,"","(Enter in sWGA Tab)")</f>
         <v>(Enter in sWGA Tab)</v>
       </c>
-      <c r="L31" s="85"/>
-      <c r="M31" s="85"/>
+      <c r="L31" s="118"/>
+      <c r="M31" s="118"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="14"/>
@@ -3354,10 +3348,10 @@
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
-      <c r="F33" s="83" t="s">
+      <c r="F33" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="83"/>
+      <c r="G33" s="116"/>
       <c r="H33"/>
     </row>
     <row r="34" spans="1:14">
@@ -3848,6 +3842,55 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="65">
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="C14:K15"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:B3"/>
@@ -3864,79 +3907,30 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="C14:K15"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="A30:J30"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C2:C4 C11:C14">
-    <cfRule type="expression" dxfId="7" priority="17">
+    <cfRule type="expression" dxfId="6" priority="17">
       <formula>COUNTIF(C2,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C8">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>COUNTIF(C7,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 F33">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>COUNTIF(D17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:L27">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$J20="-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:M32">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>LEN($K30)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3992,8 +3986,8 @@
   </sheetPr>
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -4012,28 +4006,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="E1" s="123" t="s">
+      <c r="E1" s="127" t="s">
         <v>228</v>
       </c>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="125"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="129"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="D2" s="120" t="s">
+      <c r="D2" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="118" t="s">
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="48.75" customHeight="1">
       <c r="A3" s="49" t="s">
@@ -4094,7 +4088,7 @@
       <c r="E4" s="30"/>
       <c r="F4" s="37"/>
       <c r="G4" s="30"/>
-      <c r="H4" s="126" t="str">
+      <c r="H4" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4105,9 +4099,7 @@
         <f>IF(OR(ISBLANK(tbl_sWGA[[#This Row],[sWGA qubit '[DNA'] (ng / ul)]]),ISBLANK(tbl_sWGA[[#This Row],[sWGA Dilution Factor]])),"",SUM(tbl_sWGA[[#This Row],[sWGA qubit '[DNA'] (ng / ul)]]*tbl_sWGA[[#This Row],[sWGA Dilution Factor]]))</f>
         <v/>
       </c>
-      <c r="M4" s="40" t="s">
-        <v>229</v>
-      </c>
+      <c r="M4" s="40"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="51">
@@ -4127,7 +4119,7 @@
       <c r="E5" s="30"/>
       <c r="F5" s="37"/>
       <c r="G5" s="30"/>
-      <c r="H5" s="126" t="str">
+      <c r="H5" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4138,9 +4130,7 @@
         <f>IF(OR(ISBLANK(tbl_sWGA[[#This Row],[sWGA qubit '[DNA'] (ng / ul)]]),ISBLANK(tbl_sWGA[[#This Row],[sWGA Dilution Factor]])),"",SUM(tbl_sWGA[[#This Row],[sWGA qubit '[DNA'] (ng / ul)]]*tbl_sWGA[[#This Row],[sWGA Dilution Factor]]))</f>
         <v/>
       </c>
-      <c r="M5" s="40" t="s">
-        <v>230</v>
-      </c>
+      <c r="M5" s="40"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="51">
@@ -4160,7 +4150,7 @@
       <c r="E6" s="30"/>
       <c r="F6" s="37"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="126" t="str">
+      <c r="H6" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4191,7 +4181,7 @@
       <c r="E7" s="30"/>
       <c r="F7" s="37"/>
       <c r="G7" s="30"/>
-      <c r="H7" s="126" t="str">
+      <c r="H7" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4222,7 +4212,7 @@
       <c r="E8" s="30"/>
       <c r="F8" s="37"/>
       <c r="G8" s="30"/>
-      <c r="H8" s="126" t="str">
+      <c r="H8" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4253,7 +4243,7 @@
       <c r="E9" s="30"/>
       <c r="F9" s="37"/>
       <c r="G9" s="30"/>
-      <c r="H9" s="126" t="str">
+      <c r="H9" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4284,7 +4274,7 @@
       <c r="E10" s="30"/>
       <c r="F10" s="37"/>
       <c r="G10" s="30"/>
-      <c r="H10" s="126" t="str">
+      <c r="H10" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4315,7 +4305,7 @@
       <c r="E11" s="73"/>
       <c r="F11" s="74"/>
       <c r="G11" s="73"/>
-      <c r="H11" s="127" t="str">
+      <c r="H11" s="84" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4346,7 +4336,7 @@
       <c r="E12" s="59"/>
       <c r="F12" s="60"/>
       <c r="G12" s="59"/>
-      <c r="H12" s="128" t="str">
+      <c r="H12" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4377,7 +4367,7 @@
       <c r="E13" s="30"/>
       <c r="F13" s="37"/>
       <c r="G13" s="30"/>
-      <c r="H13" s="126" t="str">
+      <c r="H13" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4408,7 +4398,7 @@
       <c r="E14" s="30"/>
       <c r="F14" s="37"/>
       <c r="G14" s="30"/>
-      <c r="H14" s="126" t="str">
+      <c r="H14" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4439,7 +4429,7 @@
       <c r="E15" s="30"/>
       <c r="F15" s="37"/>
       <c r="G15" s="30"/>
-      <c r="H15" s="126" t="str">
+      <c r="H15" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4470,7 +4460,7 @@
       <c r="E16" s="30"/>
       <c r="F16" s="37"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="126" t="str">
+      <c r="H16" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4501,7 +4491,7 @@
       <c r="E17" s="30"/>
       <c r="F17" s="37"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="126" t="str">
+      <c r="H17" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4532,7 +4522,7 @@
       <c r="E18" s="30"/>
       <c r="F18" s="37"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="126" t="str">
+      <c r="H18" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4563,7 +4553,7 @@
       <c r="E19" s="67"/>
       <c r="F19" s="68"/>
       <c r="G19" s="67"/>
-      <c r="H19" s="129" t="str">
+      <c r="H19" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4594,7 +4584,7 @@
       <c r="E20" s="59"/>
       <c r="F20" s="60"/>
       <c r="G20" s="59"/>
-      <c r="H20" s="128" t="str">
+      <c r="H20" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4625,7 +4615,7 @@
       <c r="E21" s="30"/>
       <c r="F21" s="37"/>
       <c r="G21" s="30"/>
-      <c r="H21" s="126" t="str">
+      <c r="H21" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4656,7 +4646,7 @@
       <c r="E22" s="30"/>
       <c r="F22" s="37"/>
       <c r="G22" s="30"/>
-      <c r="H22" s="126" t="str">
+      <c r="H22" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4687,7 +4677,7 @@
       <c r="E23" s="30"/>
       <c r="F23" s="37"/>
       <c r="G23" s="30"/>
-      <c r="H23" s="126" t="str">
+      <c r="H23" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4718,7 +4708,7 @@
       <c r="E24" s="30"/>
       <c r="F24" s="37"/>
       <c r="G24" s="30"/>
-      <c r="H24" s="126" t="str">
+      <c r="H24" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4749,7 +4739,7 @@
       <c r="E25" s="30"/>
       <c r="F25" s="37"/>
       <c r="G25" s="30"/>
-      <c r="H25" s="126" t="str">
+      <c r="H25" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4780,7 +4770,7 @@
       <c r="E26" s="30"/>
       <c r="F26" s="37"/>
       <c r="G26" s="30"/>
-      <c r="H26" s="126" t="str">
+      <c r="H26" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4811,7 +4801,7 @@
       <c r="E27" s="67"/>
       <c r="F27" s="68"/>
       <c r="G27" s="67"/>
-      <c r="H27" s="129" t="str">
+      <c r="H27" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4842,7 +4832,7 @@
       <c r="E28" s="59"/>
       <c r="F28" s="60"/>
       <c r="G28" s="59"/>
-      <c r="H28" s="128" t="str">
+      <c r="H28" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4873,7 +4863,7 @@
       <c r="E29" s="30"/>
       <c r="F29" s="37"/>
       <c r="G29" s="30"/>
-      <c r="H29" s="126" t="str">
+      <c r="H29" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4904,7 +4894,7 @@
       <c r="E30" s="30"/>
       <c r="F30" s="37"/>
       <c r="G30" s="30"/>
-      <c r="H30" s="126" t="str">
+      <c r="H30" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4935,7 +4925,7 @@
       <c r="E31" s="30"/>
       <c r="F31" s="37"/>
       <c r="G31" s="30"/>
-      <c r="H31" s="126" t="str">
+      <c r="H31" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4966,7 +4956,7 @@
       <c r="E32" s="30"/>
       <c r="F32" s="37"/>
       <c r="G32" s="30"/>
-      <c r="H32" s="126" t="str">
+      <c r="H32" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -4997,7 +4987,7 @@
       <c r="E33" s="30"/>
       <c r="F33" s="37"/>
       <c r="G33" s="30"/>
-      <c r="H33" s="126" t="str">
+      <c r="H33" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5028,7 +5018,7 @@
       <c r="E34" s="30"/>
       <c r="F34" s="37"/>
       <c r="G34" s="30"/>
-      <c r="H34" s="126" t="str">
+      <c r="H34" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5059,7 +5049,7 @@
       <c r="E35" s="67"/>
       <c r="F35" s="68"/>
       <c r="G35" s="67"/>
-      <c r="H35" s="129" t="str">
+      <c r="H35" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5090,7 +5080,7 @@
       <c r="E36" s="59"/>
       <c r="F36" s="60"/>
       <c r="G36" s="59"/>
-      <c r="H36" s="128" t="str">
+      <c r="H36" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5121,7 +5111,7 @@
       <c r="E37" s="30"/>
       <c r="F37" s="37"/>
       <c r="G37" s="30"/>
-      <c r="H37" s="126" t="str">
+      <c r="H37" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5152,7 +5142,7 @@
       <c r="E38" s="30"/>
       <c r="F38" s="37"/>
       <c r="G38" s="30"/>
-      <c r="H38" s="126" t="str">
+      <c r="H38" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5183,7 +5173,7 @@
       <c r="E39" s="30"/>
       <c r="F39" s="37"/>
       <c r="G39" s="30"/>
-      <c r="H39" s="126" t="str">
+      <c r="H39" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5214,7 +5204,7 @@
       <c r="E40" s="30"/>
       <c r="F40" s="37"/>
       <c r="G40" s="30"/>
-      <c r="H40" s="126" t="str">
+      <c r="H40" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5245,7 +5235,7 @@
       <c r="E41" s="30"/>
       <c r="F41" s="37"/>
       <c r="G41" s="30"/>
-      <c r="H41" s="126" t="str">
+      <c r="H41" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5276,7 +5266,7 @@
       <c r="E42" s="30"/>
       <c r="F42" s="37"/>
       <c r="G42" s="30"/>
-      <c r="H42" s="126" t="str">
+      <c r="H42" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5307,7 +5297,7 @@
       <c r="E43" s="67"/>
       <c r="F43" s="68"/>
       <c r="G43" s="67"/>
-      <c r="H43" s="129" t="str">
+      <c r="H43" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5338,7 +5328,7 @@
       <c r="E44" s="59"/>
       <c r="F44" s="60"/>
       <c r="G44" s="59"/>
-      <c r="H44" s="128" t="str">
+      <c r="H44" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5369,7 +5359,7 @@
       <c r="E45" s="30"/>
       <c r="F45" s="37"/>
       <c r="G45" s="30"/>
-      <c r="H45" s="126" t="str">
+      <c r="H45" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5400,7 +5390,7 @@
       <c r="E46" s="30"/>
       <c r="F46" s="37"/>
       <c r="G46" s="30"/>
-      <c r="H46" s="126" t="str">
+      <c r="H46" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5431,7 +5421,7 @@
       <c r="E47" s="30"/>
       <c r="F47" s="37"/>
       <c r="G47" s="30"/>
-      <c r="H47" s="126" t="str">
+      <c r="H47" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5462,7 +5452,7 @@
       <c r="E48" s="30"/>
       <c r="F48" s="37"/>
       <c r="G48" s="30"/>
-      <c r="H48" s="126" t="str">
+      <c r="H48" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5493,7 +5483,7 @@
       <c r="E49" s="30"/>
       <c r="F49" s="37"/>
       <c r="G49" s="30"/>
-      <c r="H49" s="126" t="str">
+      <c r="H49" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5524,7 +5514,7 @@
       <c r="E50" s="30"/>
       <c r="F50" s="37"/>
       <c r="G50" s="30"/>
-      <c r="H50" s="126" t="str">
+      <c r="H50" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5555,7 +5545,7 @@
       <c r="E51" s="67"/>
       <c r="F51" s="68"/>
       <c r="G51" s="67"/>
-      <c r="H51" s="129" t="str">
+      <c r="H51" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5586,7 +5576,7 @@
       <c r="E52" s="59"/>
       <c r="F52" s="60"/>
       <c r="G52" s="59"/>
-      <c r="H52" s="128" t="str">
+      <c r="H52" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5617,7 +5607,7 @@
       <c r="E53" s="30"/>
       <c r="F53" s="37"/>
       <c r="G53" s="30"/>
-      <c r="H53" s="126" t="str">
+      <c r="H53" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5648,7 +5638,7 @@
       <c r="E54" s="30"/>
       <c r="F54" s="37"/>
       <c r="G54" s="30"/>
-      <c r="H54" s="126" t="str">
+      <c r="H54" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5679,7 +5669,7 @@
       <c r="E55" s="30"/>
       <c r="F55" s="37"/>
       <c r="G55" s="30"/>
-      <c r="H55" s="126" t="str">
+      <c r="H55" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5710,7 +5700,7 @@
       <c r="E56" s="30"/>
       <c r="F56" s="37"/>
       <c r="G56" s="30"/>
-      <c r="H56" s="126" t="str">
+      <c r="H56" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5741,7 +5731,7 @@
       <c r="E57" s="30"/>
       <c r="F57" s="37"/>
       <c r="G57" s="30"/>
-      <c r="H57" s="126" t="str">
+      <c r="H57" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5772,7 +5762,7 @@
       <c r="E58" s="30"/>
       <c r="F58" s="37"/>
       <c r="G58" s="30"/>
-      <c r="H58" s="126" t="str">
+      <c r="H58" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5803,7 +5793,7 @@
       <c r="E59" s="67"/>
       <c r="F59" s="68"/>
       <c r="G59" s="67"/>
-      <c r="H59" s="129" t="str">
+      <c r="H59" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5834,7 +5824,7 @@
       <c r="E60" s="59"/>
       <c r="F60" s="60"/>
       <c r="G60" s="59"/>
-      <c r="H60" s="128" t="str">
+      <c r="H60" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5865,7 +5855,7 @@
       <c r="E61" s="30"/>
       <c r="F61" s="37"/>
       <c r="G61" s="30"/>
-      <c r="H61" s="126" t="str">
+      <c r="H61" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5896,7 +5886,7 @@
       <c r="E62" s="30"/>
       <c r="F62" s="37"/>
       <c r="G62" s="30"/>
-      <c r="H62" s="126" t="str">
+      <c r="H62" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5927,7 +5917,7 @@
       <c r="E63" s="30"/>
       <c r="F63" s="37"/>
       <c r="G63" s="30"/>
-      <c r="H63" s="126" t="str">
+      <c r="H63" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5958,7 +5948,7 @@
       <c r="E64" s="30"/>
       <c r="F64" s="37"/>
       <c r="G64" s="30"/>
-      <c r="H64" s="126" t="str">
+      <c r="H64" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -5989,7 +5979,7 @@
       <c r="E65" s="30"/>
       <c r="F65" s="37"/>
       <c r="G65" s="30"/>
-      <c r="H65" s="126" t="str">
+      <c r="H65" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6020,7 +6010,7 @@
       <c r="E66" s="30"/>
       <c r="F66" s="37"/>
       <c r="G66" s="30"/>
-      <c r="H66" s="126" t="str">
+      <c r="H66" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6051,7 +6041,7 @@
       <c r="E67" s="67"/>
       <c r="F67" s="68"/>
       <c r="G67" s="67"/>
-      <c r="H67" s="129" t="str">
+      <c r="H67" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6082,7 +6072,7 @@
       <c r="E68" s="59"/>
       <c r="F68" s="60"/>
       <c r="G68" s="59"/>
-      <c r="H68" s="128" t="str">
+      <c r="H68" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6113,7 +6103,7 @@
       <c r="E69" s="30"/>
       <c r="F69" s="37"/>
       <c r="G69" s="30"/>
-      <c r="H69" s="126" t="str">
+      <c r="H69" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6144,7 +6134,7 @@
       <c r="E70" s="30"/>
       <c r="F70" s="37"/>
       <c r="G70" s="30"/>
-      <c r="H70" s="126" t="str">
+      <c r="H70" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6175,7 +6165,7 @@
       <c r="E71" s="30"/>
       <c r="F71" s="37"/>
       <c r="G71" s="30"/>
-      <c r="H71" s="126" t="str">
+      <c r="H71" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6206,7 +6196,7 @@
       <c r="E72" s="30"/>
       <c r="F72" s="37"/>
       <c r="G72" s="30"/>
-      <c r="H72" s="126" t="str">
+      <c r="H72" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6237,7 +6227,7 @@
       <c r="E73" s="30"/>
       <c r="F73" s="37"/>
       <c r="G73" s="30"/>
-      <c r="H73" s="126" t="str">
+      <c r="H73" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6268,7 +6258,7 @@
       <c r="E74" s="30"/>
       <c r="F74" s="37"/>
       <c r="G74" s="30"/>
-      <c r="H74" s="126" t="str">
+      <c r="H74" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6299,7 +6289,7 @@
       <c r="E75" s="67"/>
       <c r="F75" s="68"/>
       <c r="G75" s="67"/>
-      <c r="H75" s="129" t="str">
+      <c r="H75" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6330,7 +6320,7 @@
       <c r="E76" s="59"/>
       <c r="F76" s="60"/>
       <c r="G76" s="59"/>
-      <c r="H76" s="128" t="str">
+      <c r="H76" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6361,7 +6351,7 @@
       <c r="E77" s="30"/>
       <c r="F77" s="37"/>
       <c r="G77" s="30"/>
-      <c r="H77" s="126" t="str">
+      <c r="H77" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6392,7 +6382,7 @@
       <c r="E78" s="30"/>
       <c r="F78" s="37"/>
       <c r="G78" s="30"/>
-      <c r="H78" s="126" t="str">
+      <c r="H78" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6423,7 +6413,7 @@
       <c r="E79" s="30"/>
       <c r="F79" s="37"/>
       <c r="G79" s="30"/>
-      <c r="H79" s="126" t="str">
+      <c r="H79" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6454,7 +6444,7 @@
       <c r="E80" s="30"/>
       <c r="F80" s="37"/>
       <c r="G80" s="30"/>
-      <c r="H80" s="126" t="str">
+      <c r="H80" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6485,7 +6475,7 @@
       <c r="E81" s="30"/>
       <c r="F81" s="37"/>
       <c r="G81" s="30"/>
-      <c r="H81" s="126" t="str">
+      <c r="H81" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6516,7 +6506,7 @@
       <c r="E82" s="30"/>
       <c r="F82" s="37"/>
       <c r="G82" s="30"/>
-      <c r="H82" s="126" t="str">
+      <c r="H82" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6547,7 +6537,7 @@
       <c r="E83" s="67"/>
       <c r="F83" s="68"/>
       <c r="G83" s="67"/>
-      <c r="H83" s="129" t="str">
+      <c r="H83" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6578,7 +6568,7 @@
       <c r="E84" s="59"/>
       <c r="F84" s="60"/>
       <c r="G84" s="59"/>
-      <c r="H84" s="128" t="str">
+      <c r="H84" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6609,7 +6599,7 @@
       <c r="E85" s="30"/>
       <c r="F85" s="37"/>
       <c r="G85" s="30"/>
-      <c r="H85" s="126" t="str">
+      <c r="H85" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6640,7 +6630,7 @@
       <c r="E86" s="30"/>
       <c r="F86" s="37"/>
       <c r="G86" s="30"/>
-      <c r="H86" s="126" t="str">
+      <c r="H86" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6671,7 +6661,7 @@
       <c r="E87" s="30"/>
       <c r="F87" s="37"/>
       <c r="G87" s="30"/>
-      <c r="H87" s="126" t="str">
+      <c r="H87" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6702,7 +6692,7 @@
       <c r="E88" s="30"/>
       <c r="F88" s="37"/>
       <c r="G88" s="30"/>
-      <c r="H88" s="126" t="str">
+      <c r="H88" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6733,7 +6723,7 @@
       <c r="E89" s="30"/>
       <c r="F89" s="37"/>
       <c r="G89" s="30"/>
-      <c r="H89" s="126" t="str">
+      <c r="H89" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6764,7 +6754,7 @@
       <c r="E90" s="30"/>
       <c r="F90" s="37"/>
       <c r="G90" s="30"/>
-      <c r="H90" s="126" t="str">
+      <c r="H90" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6795,7 +6785,7 @@
       <c r="E91" s="67"/>
       <c r="F91" s="68"/>
       <c r="G91" s="67"/>
-      <c r="H91" s="129" t="str">
+      <c r="H91" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6826,7 +6816,7 @@
       <c r="E92" s="59"/>
       <c r="F92" s="60"/>
       <c r="G92" s="59"/>
-      <c r="H92" s="128" t="str">
+      <c r="H92" s="85" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6857,7 +6847,7 @@
       <c r="E93" s="30"/>
       <c r="F93" s="37"/>
       <c r="G93" s="30"/>
-      <c r="H93" s="126" t="str">
+      <c r="H93" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6888,7 +6878,7 @@
       <c r="E94" s="30"/>
       <c r="F94" s="37"/>
       <c r="G94" s="30"/>
-      <c r="H94" s="126" t="str">
+      <c r="H94" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6919,7 +6909,7 @@
       <c r="E95" s="30"/>
       <c r="F95" s="37"/>
       <c r="G95" s="30"/>
-      <c r="H95" s="126" t="str">
+      <c r="H95" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6950,7 +6940,7 @@
       <c r="E96" s="30"/>
       <c r="F96" s="37"/>
       <c r="G96" s="30"/>
-      <c r="H96" s="126" t="str">
+      <c r="H96" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -6981,7 +6971,7 @@
       <c r="E97" s="30"/>
       <c r="F97" s="37"/>
       <c r="G97" s="30"/>
-      <c r="H97" s="126" t="str">
+      <c r="H97" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -7012,7 +7002,7 @@
       <c r="E98" s="30"/>
       <c r="F98" s="37"/>
       <c r="G98" s="30"/>
-      <c r="H98" s="126" t="str">
+      <c r="H98" s="83" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -7043,7 +7033,7 @@
       <c r="E99" s="67"/>
       <c r="F99" s="68"/>
       <c r="G99" s="67"/>
-      <c r="H99" s="129" t="str">
+      <c r="H99" s="86" t="str">
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
@@ -7061,12 +7051,12 @@
       <c r="B100" s="18"/>
       <c r="C100" s="18"/>
       <c r="D100" s="18"/>
-      <c r="E100" s="123" t="s">
+      <c r="E100" s="127" t="s">
         <v>228</v>
       </c>
-      <c r="F100" s="124"/>
-      <c r="G100" s="124"/>
-      <c r="H100" s="125"/>
+      <c r="F100" s="128"/>
+      <c r="G100" s="128"/>
+      <c r="H100" s="129"/>
       <c r="I100" s="18">
         <v>1</v>
       </c>
@@ -7255,12 +7245,12 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D4:H99">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:K99 M4:M99">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>COUNTIF(D4,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7300,7 +7290,7 @@
   </sheetPr>
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>

</xml_diff>